<commit_message>
updated model performance dataset
</commit_message>
<xml_diff>
--- a/deep_learning/analysis/ModelPerformance.xlsx
+++ b/deep_learning/analysis/ModelPerformance.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larki\Documents\GitHub\ChildrensHealthSocialMediaASP3IRE\deep_learning\train_models\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larki\Documents\GitHub\ChildrensHealthSocialMediaASP3IRE\deep_learning\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45BEA5FE-988C-4DE4-9482-06108F7549B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43AC1E0-93D0-4DB7-A6D3-23053011138B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11004" yWindow="4644" windowWidth="28668" windowHeight="20472" xr2:uid="{2B804637-ED5F-45B2-BA74-34F80D84253F}"/>
+    <workbookView xWindow="32040" yWindow="3876" windowWidth="28668" windowHeight="20472" activeTab="1" xr2:uid="{2B804637-ED5F-45B2-BA74-34F80D84253F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ChildModel" sheetId="1" r:id="rId1"/>
+    <sheet name="PlaceModel" sheetId="2" r:id="rId2"/>
+    <sheet name="HealthModel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="33">
   <si>
     <t>category</t>
   </si>
@@ -72,9 +73,6 @@
     <t>general</t>
   </si>
   <si>
-    <t>Relaxed Model</t>
-  </si>
-  <si>
     <t>Strict Model</t>
   </si>
   <si>
@@ -96,28 +94,49 @@
     <t>Data Captured</t>
   </si>
   <si>
-    <t>filtered tweets</t>
+    <t>Text Model - Image Only Tweets</t>
   </si>
   <si>
-    <t>age</t>
+    <t>cognitive health</t>
   </si>
   <si>
-    <t>place</t>
+    <t>emotional/social</t>
   </si>
   <si>
-    <t>env</t>
+    <t>physical health</t>
   </si>
   <si>
-    <t>health</t>
+    <t>positive impact</t>
   </si>
   <si>
-    <t>n total</t>
+    <t>negative impact</t>
   </si>
   <si>
-    <t xml:space="preserve">n filtered </t>
+    <t>Hybrid Model</t>
   </si>
   <si>
-    <t>% filtered</t>
+    <t>Text Model - All Tweets</t>
+  </si>
+  <si>
+    <t>childcare/daycare</t>
+  </si>
+  <si>
+    <t>park/playground</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>neighborhood</t>
+  </si>
+  <si>
+    <t>indoor</t>
+  </si>
+  <si>
+    <t>outdoor</t>
   </si>
 </sst>
 </file>
@@ -127,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,11 +161,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -338,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -375,11 +389,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -703,13 +715,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F2504E-89FB-4F8D-9B68-BC5532C6021A}">
-  <dimension ref="A2:U43"/>
+  <dimension ref="A2:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -722,39 +734,39 @@
     <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="19"/>
     </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
-      <c r="J4" s="39" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
+      <c r="J4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="39"/>
+      <c r="S4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="41"/>
-      <c r="S4" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="T4" s="40"/>
-      <c r="U4" s="41"/>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="14" t="s">
-        <v>0</v>
+      <c r="T4" s="38"/>
+      <c r="U4" s="39"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>1</v>
@@ -769,13 +781,13 @@
         <v>4</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>18</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>0</v>
@@ -793,25 +805,25 @@
         <v>4</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="14" t="s">
-        <v>18</v>
-      </c>
       <c r="S5" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="U5" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
@@ -879,7 +891,7 @@
         <v>14.583333333333336</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
@@ -947,7 +959,7 @@
         <v>27.41935483870968</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
@@ -1015,7 +1027,7 @@
         <v>21.153846153846153</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
@@ -1083,7 +1095,7 @@
         <v>4.5454545454545485</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>5.55555555555555</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
@@ -1219,9 +1231,9 @@
         <v>14.220183486238525</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="28">
         <f>SUM(B6:B11)</f>
@@ -1252,7 +1264,7 @@
         <v>64.155251141552512</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" s="28">
         <f>SUM(K6:K11)</f>
@@ -1295,64 +1307,25 @@
         <v>15.753424657534246</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="24"/>
       <c r="H13" s="19"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="17" spans="1:21">
-      <c r="A17" s="39" t="s">
+    <row r="17" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J17" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="41"/>
-      <c r="J17" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="41"/>
-      <c r="S17" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="T17" s="40"/>
-      <c r="U17" s="41"/>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="39"/>
+    </row>
+    <row r="18" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J18" s="14" t="s">
         <v>0</v>
       </c>
@@ -1369,52 +1342,16 @@
         <v>4</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q18" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="S18" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="T18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="U18" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="4">
-        <v>275</v>
-      </c>
-      <c r="C19">
-        <v>4441</v>
-      </c>
-      <c r="D19">
-        <v>205</v>
-      </c>
-      <c r="E19" s="5">
-        <v>79</v>
-      </c>
-      <c r="F19" s="25">
-        <f>SUM(B19:C19)/SUM(B19:E19)*100</f>
-        <v>94.320000000000007</v>
-      </c>
-      <c r="G19" s="26">
-        <f>B19/SUM(B19+D19)*100</f>
-        <v>57.291666666666664</v>
-      </c>
-      <c r="H19" s="25">
-        <f>B19/SUM(B19,E19)*100</f>
-        <v>77.683615819209038</v>
-      </c>
+    </row>
+    <row r="19" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J19" s="17" t="s">
         <v>5</v>
       </c>
@@ -1442,47 +1379,8 @@
         <f>K19/SUM(K19,N19)*100</f>
         <v>64.361702127659569</v>
       </c>
-      <c r="S19" s="20">
-        <f>F19-O19</f>
-        <v>-1.2999999999999972</v>
-      </c>
-      <c r="T19" s="32">
-        <f t="shared" ref="T19:T24" si="10">G19-P19</f>
-        <v>-16.714449541284402</v>
-      </c>
-      <c r="U19" s="21">
-        <f t="shared" ref="U19:U25" si="11">H19-Q19</f>
-        <v>13.321913691549469</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="4">
-        <v>190</v>
-      </c>
-      <c r="C20">
-        <v>4683</v>
-      </c>
-      <c r="D20">
-        <v>68</v>
-      </c>
-      <c r="E20" s="5">
-        <v>59</v>
-      </c>
-      <c r="F20" s="26">
-        <f t="shared" ref="F20:F25" si="12">SUM(B20:C20)/SUM(B20:E20)*100</f>
-        <v>97.460000000000008</v>
-      </c>
-      <c r="G20" s="26">
-        <f t="shared" ref="G20:G25" si="13">B20/SUM(B20+D20)*100</f>
-        <v>73.643410852713174</v>
-      </c>
-      <c r="H20" s="26">
-        <f t="shared" ref="H20:H25" si="14">B20/SUM(B20,E20)*100</f>
-        <v>76.305220883534147</v>
-      </c>
+    </row>
+    <row r="20" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J20" s="17" t="s">
         <v>6</v>
       </c>
@@ -1499,58 +1397,19 @@
         <v>91</v>
       </c>
       <c r="O20" s="26">
-        <f t="shared" ref="O20:O25" si="15">SUM(K20:L20)/SUM(K20:N20)*100</f>
+        <f t="shared" ref="O20:O25" si="10">SUM(K20:L20)/SUM(K20:N20)*100</f>
         <v>97.44</v>
       </c>
       <c r="P20" s="26">
-        <f t="shared" ref="P20:P25" si="16">K20/SUM(K20+M20)*100</f>
+        <f t="shared" ref="P20:P25" si="11">K20/SUM(K20+M20)*100</f>
         <v>79.444444444444443</v>
       </c>
       <c r="Q20" s="26">
-        <f t="shared" ref="Q20:Q25" si="17">K20/SUM(K20,N20)*100</f>
+        <f t="shared" ref="Q20:Q25" si="12">K20/SUM(K20,N20)*100</f>
         <v>61.111111111111114</v>
       </c>
-      <c r="S20" s="22">
-        <f t="shared" ref="S20:S25" si="18">F20-O20</f>
-        <v>2.0000000000010232E-2</v>
-      </c>
-      <c r="T20" s="24">
-        <f t="shared" si="10"/>
-        <v>-5.8010335917312688</v>
-      </c>
-      <c r="U20" s="23">
-        <f t="shared" si="11"/>
-        <v>15.194109772423033</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="4">
-        <v>39</v>
-      </c>
-      <c r="C21">
-        <v>4851</v>
-      </c>
-      <c r="D21">
-        <v>49</v>
-      </c>
-      <c r="E21" s="5">
-        <v>61</v>
-      </c>
-      <c r="F21" s="26">
-        <f t="shared" si="12"/>
-        <v>97.8</v>
-      </c>
-      <c r="G21" s="26">
-        <f t="shared" si="13"/>
-        <v>44.31818181818182</v>
-      </c>
-      <c r="H21" s="26">
-        <f t="shared" si="14"/>
-        <v>39</v>
-      </c>
+    </row>
+    <row r="21" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J21" s="17" t="s">
         <v>7</v>
       </c>
@@ -1567,58 +1426,19 @@
         <v>89</v>
       </c>
       <c r="O21" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>97.94</v>
       </c>
       <c r="P21" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>58.82352941176471</v>
       </c>
       <c r="Q21" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>18.348623853211009</v>
       </c>
-      <c r="S21" s="22">
-        <f t="shared" si="18"/>
-        <v>-0.14000000000000057</v>
-      </c>
-      <c r="T21" s="24">
-        <f t="shared" si="10"/>
-        <v>-14.50534759358289</v>
-      </c>
-      <c r="U21" s="23">
-        <f t="shared" si="11"/>
-        <v>20.651376146788991</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="4">
-        <v>74</v>
-      </c>
-      <c r="C22">
-        <v>4850</v>
-      </c>
-      <c r="D22">
-        <v>27</v>
-      </c>
-      <c r="E22" s="5">
-        <v>49</v>
-      </c>
-      <c r="F22" s="26">
-        <f t="shared" si="12"/>
-        <v>98.48</v>
-      </c>
-      <c r="G22" s="26">
-        <f t="shared" si="13"/>
-        <v>73.267326732673268</v>
-      </c>
-      <c r="H22" s="26">
-        <f t="shared" si="14"/>
-        <v>60.162601626016269</v>
-      </c>
+    </row>
+    <row r="22" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J22" s="17" t="s">
         <v>8</v>
       </c>
@@ -1635,58 +1455,19 @@
         <v>56</v>
       </c>
       <c r="O22" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>98.5</v>
       </c>
       <c r="P22" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>77.38095238095238</v>
       </c>
       <c r="Q22" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>53.719008264462808</v>
       </c>
-      <c r="S22" s="22">
-        <f t="shared" si="18"/>
-        <v>-1.9999999999996021E-2</v>
-      </c>
-      <c r="T22" s="24">
-        <f t="shared" si="10"/>
-        <v>-4.1136256482791111</v>
-      </c>
-      <c r="U22" s="23">
-        <f t="shared" si="11"/>
-        <v>6.4435933615534609</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
-      <c r="A23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="4">
-        <v>145</v>
-      </c>
-      <c r="C23">
-        <v>4644</v>
-      </c>
-      <c r="D23">
-        <v>147</v>
-      </c>
-      <c r="E23" s="5">
-        <v>64</v>
-      </c>
-      <c r="F23" s="26">
-        <f t="shared" si="12"/>
-        <v>95.78</v>
-      </c>
-      <c r="G23" s="26">
-        <f t="shared" si="13"/>
-        <v>49.657534246575338</v>
-      </c>
-      <c r="H23" s="26">
-        <f t="shared" si="14"/>
-        <v>69.377990430622006</v>
-      </c>
+    </row>
+    <row r="23" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J23" s="17" t="s">
         <v>9</v>
       </c>
@@ -1703,58 +1484,19 @@
         <v>86</v>
       </c>
       <c r="O23" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>97.56</v>
       </c>
       <c r="P23" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>75</v>
       </c>
       <c r="Q23" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>55.670103092783506</v>
       </c>
-      <c r="S23" s="22">
-        <f t="shared" si="18"/>
-        <v>-1.7800000000000011</v>
-      </c>
-      <c r="T23" s="24">
-        <f t="shared" si="10"/>
-        <v>-25.342465753424662</v>
-      </c>
-      <c r="U23" s="23">
-        <f t="shared" si="11"/>
-        <v>13.7078873378385</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
-      <c r="A24" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="6">
-        <v>993</v>
-      </c>
-      <c r="C24" s="7">
-        <v>3241</v>
-      </c>
-      <c r="D24" s="7">
-        <v>466</v>
-      </c>
-      <c r="E24" s="8">
-        <v>300</v>
-      </c>
-      <c r="F24" s="27">
-        <f t="shared" si="12"/>
-        <v>84.68</v>
-      </c>
-      <c r="G24" s="26">
-        <f t="shared" si="13"/>
-        <v>68.060315284441401</v>
-      </c>
-      <c r="H24" s="27">
-        <f t="shared" si="14"/>
-        <v>76.798143851508115</v>
-      </c>
+    </row>
+    <row r="24" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J24" s="18" t="s">
         <v>10</v>
       </c>
@@ -1771,64 +1513,21 @@
         <v>376</v>
       </c>
       <c r="O24" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>85.2</v>
       </c>
       <c r="P24" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>72.340425531914903</v>
       </c>
       <c r="Q24" s="27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>71.686746987951807</v>
       </c>
-      <c r="S24" s="22">
-        <f t="shared" si="18"/>
-        <v>-0.51999999999999602</v>
-      </c>
-      <c r="T24" s="24">
-        <f t="shared" si="10"/>
-        <v>-4.2801102474735018</v>
-      </c>
-      <c r="U24" s="23">
-        <f t="shared" si="11"/>
-        <v>5.1113968635563083</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="28">
-        <f>SUM(B19:B24)</f>
-        <v>1716</v>
-      </c>
-      <c r="C25" s="28">
-        <f>SUM(C19:C24)</f>
-        <v>26710</v>
-      </c>
-      <c r="D25" s="28">
-        <f>SUM(D19:D24)</f>
-        <v>962</v>
-      </c>
-      <c r="E25" s="28">
-        <f>SUM(E19:E24)</f>
-        <v>612</v>
-      </c>
-      <c r="F25" s="29">
-        <f t="shared" si="12"/>
-        <v>94.75333333333333</v>
-      </c>
-      <c r="G25" s="29">
-        <f t="shared" si="13"/>
-        <v>64.077669902912632</v>
-      </c>
-      <c r="H25" s="27">
-        <f t="shared" si="14"/>
-        <v>73.711340206185568</v>
-      </c>
+    </row>
+    <row r="25" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J25" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K25" s="28">
         <f>SUM(K19:K24)</f>
@@ -1847,300 +1546,21 @@
         <v>832</v>
       </c>
       <c r="O25" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>95.376666666666665</v>
       </c>
       <c r="P25" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>73.381294964028783</v>
       </c>
       <c r="Q25" s="27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>64.775613886536831</v>
       </c>
-      <c r="S25" s="33">
-        <f t="shared" si="18"/>
-        <v>-0.62333333333333485</v>
-      </c>
-      <c r="T25" s="34">
-        <f>G25-P25</f>
-        <v>-9.3036250611161506</v>
-      </c>
-      <c r="U25" s="35">
-        <f t="shared" si="11"/>
-        <v>8.9357263196487366</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="G27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="G28" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29">
-        <f>B19+E19</f>
-        <v>354</v>
-      </c>
-      <c r="C29">
-        <f>C19+D19</f>
-        <v>4646</v>
-      </c>
-      <c r="D29">
-        <f>B29/(B29+C29)*100</f>
-        <v>7.08</v>
-      </c>
-      <c r="E29">
-        <f>100-D29</f>
-        <v>92.92</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2864352</v>
-      </c>
-      <c r="I29" s="2">
-        <v>660577</v>
-      </c>
-      <c r="J29" s="21">
-        <f>I29/H29*100</f>
-        <v>23.062004949112399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30">
-        <f t="shared" ref="B30:B35" si="19">B20+E20</f>
-        <v>249</v>
-      </c>
-      <c r="C30">
-        <f t="shared" ref="C30:C35" si="20">C20+D20</f>
-        <v>4751</v>
-      </c>
-      <c r="D30">
-        <f t="shared" ref="D30:D35" si="21">B30/(B30+C30)*100</f>
-        <v>4.9799999999999995</v>
-      </c>
-      <c r="E30">
-        <f t="shared" ref="E30:E35" si="22">100-D30</f>
-        <v>95.02</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="4">
-        <v>4763240</v>
-      </c>
-      <c r="I30">
-        <v>374660</v>
-      </c>
-      <c r="J30" s="23">
-        <f>I30/H30*100</f>
-        <v>7.8656544704864757</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="20"/>
-        <v>4900</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="22"/>
-        <v>98</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="4">
-        <f>7169193+8186156</f>
-        <v>15355349</v>
-      </c>
-      <c r="I31">
-        <f>245364+265503</f>
-        <v>510867</v>
-      </c>
-      <c r="J31" s="23">
-        <f>I31/H31*100</f>
-        <v>3.3269644343479268</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="A32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="19"/>
-        <v>123</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="20"/>
-        <v>4877</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="21"/>
-        <v>2.46</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="22"/>
-        <v>97.54</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="4">
-        <v>1071152</v>
-      </c>
-      <c r="I32">
-        <v>20392</v>
-      </c>
-      <c r="J32" s="23">
-        <f t="shared" ref="J32:J33" si="23">I32/H32*100</f>
-        <v>1.9037447533123217</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="19"/>
-        <v>209</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="20"/>
-        <v>4791</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="21"/>
-        <v>4.18</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="22"/>
-        <v>95.82</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="37">
-        <v>19483815.330000002</v>
-      </c>
-      <c r="I33" s="7">
-        <f>1190437</f>
-        <v>1190437</v>
-      </c>
-      <c r="J33" s="38">
-        <f t="shared" si="23"/>
-        <v>6.1098762220715415</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="19"/>
-        <v>1293</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="20"/>
-        <v>3707</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="21"/>
-        <v>25.86</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="22"/>
-        <v>74.14</v>
-      </c>
-      <c r="G34">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="19"/>
-        <v>2328</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="20"/>
-        <v>27672</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="21"/>
-        <v>7.76</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="22"/>
-        <v>92.24</v>
-      </c>
-      <c r="G35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35">
-        <v>94092</v>
-      </c>
-      <c r="I35">
-        <v>6325</v>
-      </c>
-      <c r="J35" s="24">
-        <f>I35/H35*100</f>
-        <v>6.7221442843174755</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="G39" s="36"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="G40" s="36"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="G41" s="36"/>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="G42" s="36"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="G43" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A17:H17"/>
+  <mergeCells count="4">
     <mergeCell ref="J17:Q17"/>
-    <mergeCell ref="S17:U17"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="J4:Q4"/>
     <mergeCell ref="A4:H4"/>
@@ -2152,12 +1572,1941 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC10C75C-1D20-4666-BCBB-B7233EA77D40}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:U25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
+      <c r="J2" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
+      <c r="S2" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="38"/>
+      <c r="U2" s="39"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>955</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>35</v>
+      </c>
+      <c r="F4" s="25">
+        <f>SUM(B4:C4)/SUM(B4:E4)*100</f>
+        <v>96.464646464646464</v>
+      </c>
+      <c r="G4" s="26">
+        <v>0</v>
+      </c>
+      <c r="H4" s="25">
+        <f>B4/SUM(B4,E4)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="4">
+        <v>13</v>
+      </c>
+      <c r="L4">
+        <v>950</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>22</v>
+      </c>
+      <c r="O4" s="25">
+        <f>SUM(K4:L4)/SUM(K4:N4)*100</f>
+        <v>97.27272727272728</v>
+      </c>
+      <c r="P4" s="26">
+        <f>K4/SUM(K4+M4)*100</f>
+        <v>72.222222222222214</v>
+      </c>
+      <c r="Q4" s="25">
+        <f>K4/SUM(K4,N4)*100</f>
+        <v>37.142857142857146</v>
+      </c>
+      <c r="S4" s="20">
+        <f>F4-O4</f>
+        <v>-0.80808080808081684</v>
+      </c>
+      <c r="T4" s="32">
+        <f t="shared" ref="T4:U11" si="0">G4-P4</f>
+        <v>-72.222222222222214</v>
+      </c>
+      <c r="U4" s="21">
+        <f t="shared" si="0"/>
+        <v>-37.142857142857146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>937</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>53</v>
+      </c>
+      <c r="F5" s="26">
+        <f t="shared" ref="F5:F11" si="1">SUM(B5:C5)/SUM(B5:E5)*100</f>
+        <v>94.646464646464651</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0</v>
+      </c>
+      <c r="H5" s="26">
+        <f t="shared" ref="H5:H11" si="2">B5/SUM(B5,E5)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="4">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>931</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>23</v>
+      </c>
+      <c r="O5" s="26">
+        <f t="shared" ref="O5:O11" si="3">SUM(K5:L5)/SUM(K5:N5)*100</f>
+        <v>97.070707070707073</v>
+      </c>
+      <c r="P5" s="26">
+        <f t="shared" ref="P5:P11" si="4">K5/SUM(K5+M5)*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="Q5" s="26">
+        <f t="shared" ref="Q5:Q11" si="5">K5/SUM(K5,N5)*100</f>
+        <v>56.60377358490566</v>
+      </c>
+      <c r="S5" s="22">
+        <f t="shared" ref="S5:S11" si="6">F5-O5</f>
+        <v>-2.4242424242424221</v>
+      </c>
+      <c r="T5" s="24">
+        <f t="shared" si="0"/>
+        <v>-83.333333333333343</v>
+      </c>
+      <c r="U5" s="23">
+        <f t="shared" si="0"/>
+        <v>-56.60377358490566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>765</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>225</v>
+      </c>
+      <c r="F6" s="26">
+        <f t="shared" si="1"/>
+        <v>77.272727272727266</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0</v>
+      </c>
+      <c r="H6" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="4">
+        <v>127</v>
+      </c>
+      <c r="L6">
+        <v>727</v>
+      </c>
+      <c r="M6">
+        <v>38</v>
+      </c>
+      <c r="N6">
+        <v>98</v>
+      </c>
+      <c r="O6" s="26">
+        <f t="shared" si="3"/>
+        <v>86.26262626262627</v>
+      </c>
+      <c r="P6" s="26">
+        <f t="shared" si="4"/>
+        <v>76.969696969696969</v>
+      </c>
+      <c r="Q6" s="26">
+        <f t="shared" si="5"/>
+        <v>56.444444444444443</v>
+      </c>
+      <c r="S6" s="22">
+        <f t="shared" si="6"/>
+        <v>-8.9898989898990038</v>
+      </c>
+      <c r="T6" s="24">
+        <f t="shared" si="0"/>
+        <v>-76.969696969696969</v>
+      </c>
+      <c r="U6" s="23">
+        <f t="shared" si="0"/>
+        <v>-56.444444444444443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>849</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>141</v>
+      </c>
+      <c r="F7" s="26">
+        <f t="shared" si="1"/>
+        <v>85.757575757575751</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0</v>
+      </c>
+      <c r="H7" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="4">
+        <v>92</v>
+      </c>
+      <c r="L7">
+        <v>809</v>
+      </c>
+      <c r="M7">
+        <v>40</v>
+      </c>
+      <c r="N7">
+        <v>49</v>
+      </c>
+      <c r="O7" s="26">
+        <f t="shared" si="3"/>
+        <v>91.01010101010101</v>
+      </c>
+      <c r="P7" s="26">
+        <f t="shared" si="4"/>
+        <v>69.696969696969703</v>
+      </c>
+      <c r="Q7" s="26">
+        <f t="shared" si="5"/>
+        <v>65.248226950354621</v>
+      </c>
+      <c r="S7" s="22">
+        <f t="shared" si="6"/>
+        <v>-5.2525252525252597</v>
+      </c>
+      <c r="T7" s="24">
+        <f t="shared" si="0"/>
+        <v>-69.696969696969703</v>
+      </c>
+      <c r="U7" s="23">
+        <f t="shared" si="0"/>
+        <v>-65.248226950354621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>969</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>21</v>
+      </c>
+      <c r="F8" s="26">
+        <f t="shared" si="1"/>
+        <v>97.878787878787875</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0</v>
+      </c>
+      <c r="H8" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="4">
+        <v>9</v>
+      </c>
+      <c r="L8">
+        <v>960</v>
+      </c>
+      <c r="M8">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <v>12</v>
+      </c>
+      <c r="O8" s="26">
+        <f t="shared" si="3"/>
+        <v>97.878787878787875</v>
+      </c>
+      <c r="P8" s="26">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="Q8" s="26">
+        <f t="shared" si="5"/>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="S8" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="24">
+        <f t="shared" si="0"/>
+        <v>-50</v>
+      </c>
+      <c r="U8" s="23">
+        <f t="shared" si="0"/>
+        <v>-42.857142857142854</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1">
+        <v>155</v>
+      </c>
+      <c r="C9" s="2">
+        <v>476</v>
+      </c>
+      <c r="D9" s="2">
+        <v>49</v>
+      </c>
+      <c r="E9" s="3">
+        <v>310</v>
+      </c>
+      <c r="F9" s="25">
+        <f t="shared" si="1"/>
+        <v>63.737373737373737</v>
+      </c>
+      <c r="G9" s="25">
+        <f t="shared" ref="G9:G11" si="7">B9/SUM(B9+D9)*100</f>
+        <v>75.980392156862735</v>
+      </c>
+      <c r="H9" s="25">
+        <f t="shared" si="2"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="1">
+        <v>317</v>
+      </c>
+      <c r="L9" s="2">
+        <v>376</v>
+      </c>
+      <c r="M9" s="2">
+        <v>149</v>
+      </c>
+      <c r="N9" s="2">
+        <v>148</v>
+      </c>
+      <c r="O9" s="25">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="P9" s="25">
+        <f t="shared" si="4"/>
+        <v>68.02575107296137</v>
+      </c>
+      <c r="Q9" s="25">
+        <f t="shared" si="5"/>
+        <v>68.172043010752688</v>
+      </c>
+      <c r="S9" s="22">
+        <f t="shared" si="6"/>
+        <v>-6.262626262626263</v>
+      </c>
+      <c r="T9" s="24">
+        <f t="shared" si="0"/>
+        <v>7.9546410839013646</v>
+      </c>
+      <c r="U9" s="23">
+        <f t="shared" si="0"/>
+        <v>-34.838709677419359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6">
+        <v>230</v>
+      </c>
+      <c r="C10" s="7">
+        <v>515</v>
+      </c>
+      <c r="D10" s="7">
+        <v>154</v>
+      </c>
+      <c r="E10" s="8">
+        <v>91</v>
+      </c>
+      <c r="F10" s="27">
+        <f t="shared" si="1"/>
+        <v>75.252525252525245</v>
+      </c>
+      <c r="G10" s="26">
+        <f t="shared" ref="G10" si="8">B10/SUM(B10+D10)*100</f>
+        <v>59.895833333333336</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="2"/>
+        <v>71.651090342679126</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="7">
+        <v>202</v>
+      </c>
+      <c r="L10" s="7">
+        <v>605</v>
+      </c>
+      <c r="M10" s="7">
+        <v>64</v>
+      </c>
+      <c r="N10" s="7">
+        <v>119</v>
+      </c>
+      <c r="O10" s="27">
+        <f t="shared" si="3"/>
+        <v>81.515151515151516</v>
+      </c>
+      <c r="P10" s="26">
+        <f t="shared" si="4"/>
+        <v>75.939849624060145</v>
+      </c>
+      <c r="Q10" s="27">
+        <f t="shared" si="5"/>
+        <v>62.928348909657316</v>
+      </c>
+      <c r="S10" s="22">
+        <f t="shared" si="6"/>
+        <v>-6.2626262626262701</v>
+      </c>
+      <c r="T10" s="24">
+        <f t="shared" si="0"/>
+        <v>-16.044016290726809</v>
+      </c>
+      <c r="U10" s="23">
+        <f t="shared" si="0"/>
+        <v>8.7227414330218096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="28">
+        <f>SUM(B4:B10)</f>
+        <v>385</v>
+      </c>
+      <c r="C11" s="28">
+        <f>SUM(C4:C10)</f>
+        <v>5466</v>
+      </c>
+      <c r="D11" s="28">
+        <f>SUM(D4:D10)</f>
+        <v>203</v>
+      </c>
+      <c r="E11" s="28">
+        <f>SUM(E4:E10)</f>
+        <v>876</v>
+      </c>
+      <c r="F11" s="29">
+        <f t="shared" si="1"/>
+        <v>84.430014430014438</v>
+      </c>
+      <c r="G11" s="29">
+        <f t="shared" si="7"/>
+        <v>65.476190476190482</v>
+      </c>
+      <c r="H11" s="27">
+        <f t="shared" si="2"/>
+        <v>30.531324345757337</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="28">
+        <f>SUM(K4:K10)</f>
+        <v>790</v>
+      </c>
+      <c r="L11" s="28">
+        <f>SUM(L4:L10)</f>
+        <v>5358</v>
+      </c>
+      <c r="M11" s="28">
+        <f>SUM(M4:M10)</f>
+        <v>311</v>
+      </c>
+      <c r="N11" s="30">
+        <f>SUM(N4:N10)</f>
+        <v>471</v>
+      </c>
+      <c r="O11" s="27">
+        <f t="shared" si="3"/>
+        <v>88.715728715728716</v>
+      </c>
+      <c r="P11" s="29">
+        <f t="shared" si="4"/>
+        <v>71.752951861943686</v>
+      </c>
+      <c r="Q11" s="27">
+        <f t="shared" si="5"/>
+        <v>62.648691514670894</v>
+      </c>
+      <c r="S11" s="33">
+        <f t="shared" si="6"/>
+        <v>-4.2857142857142776</v>
+      </c>
+      <c r="T11" s="34">
+        <f t="shared" si="0"/>
+        <v>-6.2767613857532041</v>
+      </c>
+      <c r="U11" s="35">
+        <f t="shared" si="0"/>
+        <v>-32.11736716891356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="24"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="J16" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="39"/>
+      <c r="S16" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="38"/>
+      <c r="U16" s="39"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="S17" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="4">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>950</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>18</v>
+      </c>
+      <c r="F18" s="25">
+        <f>SUM(B18:C18)/SUM(B18:E18)*100</f>
+        <v>97.676767676767668</v>
+      </c>
+      <c r="G18" s="26">
+        <f>B18/SUM(B18+D18)*100</f>
+        <v>77.272727272727266</v>
+      </c>
+      <c r="H18" s="25">
+        <f>B18/SUM(B18,E18)*100</f>
+        <v>48.571428571428569</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="4">
+        <v>82</v>
+      </c>
+      <c r="L18">
+        <v>4797</v>
+      </c>
+      <c r="M18">
+        <v>44</v>
+      </c>
+      <c r="N18">
+        <v>77</v>
+      </c>
+      <c r="O18" s="25">
+        <f>SUM(K18:L18)/SUM(K18:N18)*100</f>
+        <v>97.58</v>
+      </c>
+      <c r="P18" s="26">
+        <f>K18/SUM(K18+M18)*100</f>
+        <v>65.079365079365076</v>
+      </c>
+      <c r="Q18" s="25">
+        <f>K18/SUM(K18,N18)*100</f>
+        <v>51.572327044025158</v>
+      </c>
+      <c r="S18" s="20">
+        <f>F18-O18</f>
+        <v>9.6767676767669286E-2</v>
+      </c>
+      <c r="T18" s="32">
+        <f t="shared" ref="T18:U24" si="9">G18-P18</f>
+        <v>12.193362193362191</v>
+      </c>
+      <c r="U18" s="21">
+        <f t="shared" si="9"/>
+        <v>-3.0008984725965888</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>930</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>21</v>
+      </c>
+      <c r="F19" s="26">
+        <f t="shared" ref="F19:F25" si="10">SUM(B19:C19)/SUM(B19:E19)*100</f>
+        <v>97.171717171717177</v>
+      </c>
+      <c r="G19" s="26">
+        <f t="shared" ref="G19:G25" si="11">B19/SUM(B19+D19)*100</f>
+        <v>82.051282051282044</v>
+      </c>
+      <c r="H19" s="26">
+        <f t="shared" ref="H19:H25" si="12">B19/SUM(B19,E19)*100</f>
+        <v>60.377358490566039</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="4">
+        <v>123</v>
+      </c>
+      <c r="L19">
+        <v>4764</v>
+      </c>
+      <c r="M19">
+        <v>37</v>
+      </c>
+      <c r="N19">
+        <v>76</v>
+      </c>
+      <c r="O19" s="26">
+        <f t="shared" ref="O19:O25" si="13">SUM(K19:L19)/SUM(K19:N19)*100</f>
+        <v>97.740000000000009</v>
+      </c>
+      <c r="P19" s="26">
+        <f t="shared" ref="P19:P25" si="14">K19/SUM(K19+M19)*100</f>
+        <v>76.875</v>
+      </c>
+      <c r="Q19" s="26">
+        <f t="shared" ref="Q19:Q25" si="15">K19/SUM(K19,N19)*100</f>
+        <v>61.809045226130657</v>
+      </c>
+      <c r="S19" s="22">
+        <f t="shared" ref="S19:S24" si="16">F19-O19</f>
+        <v>-0.5682828282828325</v>
+      </c>
+      <c r="T19" s="24">
+        <f t="shared" si="9"/>
+        <v>5.176282051282044</v>
+      </c>
+      <c r="U19" s="23">
+        <f t="shared" si="9"/>
+        <v>-1.4316867355646181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="4">
+        <v>147</v>
+      </c>
+      <c r="C20">
+        <v>712</v>
+      </c>
+      <c r="D20">
+        <v>53</v>
+      </c>
+      <c r="E20">
+        <v>78</v>
+      </c>
+      <c r="F20" s="26">
+        <f t="shared" si="10"/>
+        <v>86.767676767676775</v>
+      </c>
+      <c r="G20" s="26">
+        <f t="shared" si="11"/>
+        <v>73.5</v>
+      </c>
+      <c r="H20" s="26">
+        <f t="shared" si="12"/>
+        <v>65.333333333333329</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="4">
+        <v>508</v>
+      </c>
+      <c r="L20">
+        <v>4094</v>
+      </c>
+      <c r="M20">
+        <v>214</v>
+      </c>
+      <c r="N20">
+        <v>184</v>
+      </c>
+      <c r="O20" s="26">
+        <f t="shared" si="13"/>
+        <v>92.04</v>
+      </c>
+      <c r="P20" s="26">
+        <f t="shared" si="14"/>
+        <v>70.360110803324105</v>
+      </c>
+      <c r="Q20" s="26">
+        <f t="shared" si="15"/>
+        <v>73.410404624277461</v>
+      </c>
+      <c r="S20" s="22">
+        <f t="shared" si="16"/>
+        <v>-5.272323232323231</v>
+      </c>
+      <c r="T20" s="24">
+        <f t="shared" si="9"/>
+        <v>3.1398891966758953</v>
+      </c>
+      <c r="U20" s="23">
+        <f t="shared" si="9"/>
+        <v>-8.0770712909441329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4">
+        <v>95</v>
+      </c>
+      <c r="C21">
+        <v>814</v>
+      </c>
+      <c r="D21">
+        <v>35</v>
+      </c>
+      <c r="E21">
+        <v>46</v>
+      </c>
+      <c r="F21" s="26">
+        <f t="shared" si="10"/>
+        <v>91.818181818181827</v>
+      </c>
+      <c r="G21" s="26">
+        <f t="shared" si="11"/>
+        <v>73.076923076923066</v>
+      </c>
+      <c r="H21" s="26">
+        <f t="shared" si="12"/>
+        <v>67.37588652482269</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" s="4">
+        <v>374</v>
+      </c>
+      <c r="L21">
+        <v>4273</v>
+      </c>
+      <c r="M21">
+        <v>167</v>
+      </c>
+      <c r="N21">
+        <v>186</v>
+      </c>
+      <c r="O21" s="26">
+        <f t="shared" si="13"/>
+        <v>92.94</v>
+      </c>
+      <c r="P21" s="26">
+        <f t="shared" si="14"/>
+        <v>69.131238447319774</v>
+      </c>
+      <c r="Q21" s="26">
+        <f t="shared" si="15"/>
+        <v>66.785714285714278</v>
+      </c>
+      <c r="S21" s="22">
+        <f t="shared" si="16"/>
+        <v>-1.1218181818181705</v>
+      </c>
+      <c r="T21" s="24">
+        <f t="shared" si="9"/>
+        <v>3.9456846296032921</v>
+      </c>
+      <c r="U21" s="23">
+        <f t="shared" si="9"/>
+        <v>0.5901722391084121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>964</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>14</v>
+      </c>
+      <c r="F22" s="26">
+        <f t="shared" si="10"/>
+        <v>98.080808080808083</v>
+      </c>
+      <c r="G22" s="26">
+        <f t="shared" si="11"/>
+        <v>58.333333333333336</v>
+      </c>
+      <c r="H22" s="26">
+        <f t="shared" si="12"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="4">
+        <v>40</v>
+      </c>
+      <c r="L22">
+        <v>4865</v>
+      </c>
+      <c r="M22">
+        <v>23</v>
+      </c>
+      <c r="N22">
+        <v>72</v>
+      </c>
+      <c r="O22" s="26">
+        <f t="shared" si="13"/>
+        <v>98.1</v>
+      </c>
+      <c r="P22" s="26">
+        <f t="shared" si="14"/>
+        <v>63.492063492063487</v>
+      </c>
+      <c r="Q22" s="26">
+        <f t="shared" si="15"/>
+        <v>35.714285714285715</v>
+      </c>
+      <c r="S22" s="22">
+        <f t="shared" si="16"/>
+        <v>-1.9191919191911211E-2</v>
+      </c>
+      <c r="T22" s="24">
+        <f t="shared" si="9"/>
+        <v>-5.1587301587301511</v>
+      </c>
+      <c r="U22" s="23">
+        <f t="shared" si="9"/>
+        <v>-2.3809523809523867</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1">
+        <v>363</v>
+      </c>
+      <c r="C23" s="2">
+        <v>407</v>
+      </c>
+      <c r="D23" s="2">
+        <v>118</v>
+      </c>
+      <c r="E23" s="2">
+        <v>102</v>
+      </c>
+      <c r="F23" s="25">
+        <f t="shared" si="10"/>
+        <v>77.777777777777786</v>
+      </c>
+      <c r="G23" s="25">
+        <f t="shared" si="11"/>
+        <v>75.467775467775468</v>
+      </c>
+      <c r="H23" s="25">
+        <f t="shared" si="12"/>
+        <v>78.064516129032256</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1239</v>
+      </c>
+      <c r="L23" s="2">
+        <v>2835</v>
+      </c>
+      <c r="M23" s="2">
+        <v>488</v>
+      </c>
+      <c r="N23" s="2">
+        <v>438</v>
+      </c>
+      <c r="O23" s="25">
+        <f t="shared" si="13"/>
+        <v>81.47999999999999</v>
+      </c>
+      <c r="P23" s="25">
+        <f t="shared" si="14"/>
+        <v>71.742906774753905</v>
+      </c>
+      <c r="Q23" s="25">
+        <f t="shared" si="15"/>
+        <v>73.881932021466895</v>
+      </c>
+      <c r="S23" s="22">
+        <f t="shared" si="16"/>
+        <v>-3.7022222222222041</v>
+      </c>
+      <c r="T23" s="24">
+        <f t="shared" si="9"/>
+        <v>3.7248686930215626</v>
+      </c>
+      <c r="U23" s="23">
+        <f t="shared" si="9"/>
+        <v>4.1825841075653614</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="7">
+        <v>245</v>
+      </c>
+      <c r="C24" s="7">
+        <v>605</v>
+      </c>
+      <c r="D24" s="7">
+        <v>64</v>
+      </c>
+      <c r="E24" s="7">
+        <v>76</v>
+      </c>
+      <c r="F24" s="27">
+        <f t="shared" si="10"/>
+        <v>85.858585858585855</v>
+      </c>
+      <c r="G24" s="26">
+        <f t="shared" si="11"/>
+        <v>79.288025889967642</v>
+      </c>
+      <c r="H24" s="27">
+        <f t="shared" si="12"/>
+        <v>76.323987538940813</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" s="7">
+        <v>539</v>
+      </c>
+      <c r="L24" s="7">
+        <v>3966</v>
+      </c>
+      <c r="M24" s="7">
+        <v>226</v>
+      </c>
+      <c r="N24" s="7">
+        <v>269</v>
+      </c>
+      <c r="O24" s="27">
+        <f t="shared" si="13"/>
+        <v>90.100000000000009</v>
+      </c>
+      <c r="P24" s="26">
+        <f t="shared" si="14"/>
+        <v>70.457516339869287</v>
+      </c>
+      <c r="Q24" s="27">
+        <f t="shared" si="15"/>
+        <v>66.707920792079207</v>
+      </c>
+      <c r="S24" s="33">
+        <f t="shared" si="16"/>
+        <v>-4.241414141414154</v>
+      </c>
+      <c r="T24" s="34">
+        <f>G24-P24</f>
+        <v>8.8305095500983555</v>
+      </c>
+      <c r="U24" s="35">
+        <f t="shared" si="9"/>
+        <v>9.6160667468616055</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="28">
+        <f>SUM(B18:B24)</f>
+        <v>906</v>
+      </c>
+      <c r="C25" s="28">
+        <f>SUM(C18:C24)</f>
+        <v>5382</v>
+      </c>
+      <c r="D25" s="28">
+        <f>SUM(D18:D24)</f>
+        <v>287</v>
+      </c>
+      <c r="E25" s="30">
+        <f>SUM(E18:E24)</f>
+        <v>355</v>
+      </c>
+      <c r="F25" s="27">
+        <f t="shared" si="10"/>
+        <v>90.735930735930737</v>
+      </c>
+      <c r="G25" s="29">
+        <f t="shared" si="11"/>
+        <v>75.943000838222957</v>
+      </c>
+      <c r="H25" s="27">
+        <f t="shared" si="12"/>
+        <v>71.847739888977003</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="28">
+        <f>SUM(K18:K24)</f>
+        <v>2905</v>
+      </c>
+      <c r="L25" s="28">
+        <f>SUM(L18:L24)</f>
+        <v>29594</v>
+      </c>
+      <c r="M25" s="28">
+        <f>SUM(M18:M24)</f>
+        <v>1199</v>
+      </c>
+      <c r="N25" s="30">
+        <f>SUM(N18:N24)</f>
+        <v>1302</v>
+      </c>
+      <c r="O25" s="27">
+        <f t="shared" si="13"/>
+        <v>92.854285714285709</v>
+      </c>
+      <c r="P25" s="29">
+        <f t="shared" si="14"/>
+        <v>70.784600389863556</v>
+      </c>
+      <c r="Q25" s="27">
+        <f t="shared" si="15"/>
+        <v>69.051580698835281</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="J16:Q16"/>
+    <mergeCell ref="S16:U16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9270B70-B62F-4F97-B8C2-FDA91DC787F3}">
+  <dimension ref="A2:Q21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
+      <c r="J2" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>753</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>28</v>
+      </c>
+      <c r="F4" s="25">
+        <f>SUM(B4:C4)/SUM(B4:E4)*100</f>
+        <v>96.414852752880918</v>
+      </c>
+      <c r="G4" s="26">
+        <v>0</v>
+      </c>
+      <c r="H4" s="25">
+        <f>B4/SUM(B4,E4)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>749</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>24</v>
+      </c>
+      <c r="O4" s="25">
+        <f>SUM(K4:L4)/SUM(K4:N4)*100</f>
+        <v>96.414852752880918</v>
+      </c>
+      <c r="P4" s="26">
+        <f>K4/SUM(K4+M4)*100</f>
+        <v>50</v>
+      </c>
+      <c r="Q4" s="25">
+        <f>K4/SUM(K4,N4)*100</f>
+        <v>14.285714285714285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>580</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>201</v>
+      </c>
+      <c r="F5" s="26">
+        <f t="shared" ref="F5:F9" si="0">SUM(B5:C5)/SUM(B5:E5)*100</f>
+        <v>74.263764404609475</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0</v>
+      </c>
+      <c r="H5" s="26">
+        <f t="shared" ref="H5:H9" si="1">B5/SUM(B5,E5)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="4">
+        <v>72</v>
+      </c>
+      <c r="L5">
+        <v>538</v>
+      </c>
+      <c r="M5">
+        <v>42</v>
+      </c>
+      <c r="N5">
+        <v>129</v>
+      </c>
+      <c r="O5" s="26">
+        <f t="shared" ref="O5:O9" si="2">SUM(K5:L5)/SUM(K5:N5)*100</f>
+        <v>78.104993597951349</v>
+      </c>
+      <c r="P5" s="26">
+        <f t="shared" ref="P5:P9" si="3">K5/SUM(K5+M5)*100</f>
+        <v>63.157894736842103</v>
+      </c>
+      <c r="Q5" s="26">
+        <f t="shared" ref="Q5:Q9" si="4">K5/SUM(K5,N5)*100</f>
+        <v>35.820895522388057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6">
+        <v>134</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>645</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="27">
+        <f t="shared" si="0"/>
+        <v>17.285531370038413</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0</v>
+      </c>
+      <c r="H6" s="27">
+        <f t="shared" si="1"/>
+        <v>99.259259259259252</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="6">
+        <v>100</v>
+      </c>
+      <c r="L6" s="7">
+        <v>617</v>
+      </c>
+      <c r="M6" s="7">
+        <v>29</v>
+      </c>
+      <c r="N6" s="7">
+        <v>35</v>
+      </c>
+      <c r="O6" s="27">
+        <f t="shared" si="2"/>
+        <v>91.805377720870666</v>
+      </c>
+      <c r="P6" s="27">
+        <f t="shared" si="3"/>
+        <v>77.51937984496125</v>
+      </c>
+      <c r="Q6" s="27">
+        <f t="shared" si="4"/>
+        <v>74.074074074074076</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4">
+        <v>171</v>
+      </c>
+      <c r="C7">
+        <v>103</v>
+      </c>
+      <c r="D7">
+        <v>474</v>
+      </c>
+      <c r="E7" s="5">
+        <v>33</v>
+      </c>
+      <c r="F7" s="26">
+        <f t="shared" si="0"/>
+        <v>35.083226632522404</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0</v>
+      </c>
+      <c r="H7" s="26">
+        <f t="shared" si="1"/>
+        <v>83.82352941176471</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="4">
+        <v>87</v>
+      </c>
+      <c r="L7">
+        <v>533</v>
+      </c>
+      <c r="M7">
+        <v>44</v>
+      </c>
+      <c r="N7">
+        <v>117</v>
+      </c>
+      <c r="O7" s="26">
+        <f t="shared" si="2"/>
+        <v>79.385403329065298</v>
+      </c>
+      <c r="P7" s="26">
+        <f t="shared" si="3"/>
+        <v>66.412213740458014</v>
+      </c>
+      <c r="Q7" s="26">
+        <f t="shared" si="4"/>
+        <v>42.647058823529413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>651</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>129</v>
+      </c>
+      <c r="F8" s="26">
+        <f t="shared" si="0"/>
+        <v>83.354673495518554</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="6">
+        <v>88</v>
+      </c>
+      <c r="L8" s="7">
+        <v>610</v>
+      </c>
+      <c r="M8" s="7">
+        <v>42</v>
+      </c>
+      <c r="N8" s="7">
+        <v>41</v>
+      </c>
+      <c r="O8" s="27">
+        <f t="shared" si="2"/>
+        <v>89.372599231754151</v>
+      </c>
+      <c r="P8" s="27">
+        <f t="shared" si="3"/>
+        <v>67.692307692307693</v>
+      </c>
+      <c r="Q8" s="27">
+        <f t="shared" si="4"/>
+        <v>68.217054263565885</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="28">
+        <f>SUM(B4:B8)</f>
+        <v>305</v>
+      </c>
+      <c r="C9" s="28">
+        <f>SUM(C4:C8)</f>
+        <v>2088</v>
+      </c>
+      <c r="D9" s="28">
+        <f>SUM(D4:D8)</f>
+        <v>1120</v>
+      </c>
+      <c r="E9" s="28">
+        <f>SUM(E4:E8)</f>
+        <v>392</v>
+      </c>
+      <c r="F9" s="29">
+        <f t="shared" si="0"/>
+        <v>61.280409731113963</v>
+      </c>
+      <c r="G9" s="29">
+        <f t="shared" ref="G9" si="5">B9/SUM(B9+D9)*100</f>
+        <v>21.403508771929825</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="1"/>
+        <v>43.758967001434719</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7">
+        <f>SUM(K4:K8)</f>
+        <v>351</v>
+      </c>
+      <c r="L9" s="7">
+        <f>SUM(L4:L8)</f>
+        <v>3047</v>
+      </c>
+      <c r="M9" s="7">
+        <f>SUM(M4:M8)</f>
+        <v>161</v>
+      </c>
+      <c r="N9" s="8">
+        <f>SUM(N4:N8)</f>
+        <v>346</v>
+      </c>
+      <c r="O9" s="27">
+        <f t="shared" si="2"/>
+        <v>87.016645326504488</v>
+      </c>
+      <c r="P9" s="27">
+        <f t="shared" si="3"/>
+        <v>68.5546875</v>
+      </c>
+      <c r="Q9" s="27">
+        <f t="shared" si="4"/>
+        <v>50.358680057388803</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="24"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J14" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="39"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J15" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="4">
+        <v>73</v>
+      </c>
+      <c r="L16">
+        <v>4276</v>
+      </c>
+      <c r="M16">
+        <v>29</v>
+      </c>
+      <c r="N16">
+        <v>172</v>
+      </c>
+      <c r="O16" s="25">
+        <f>SUM(K16:L16)/SUM(K16:N16)*100</f>
+        <v>95.582417582417577</v>
+      </c>
+      <c r="P16" s="26">
+        <f>K16/SUM(K16+M16)*100</f>
+        <v>71.568627450980387</v>
+      </c>
+      <c r="Q16" s="25">
+        <f>K16/SUM(K16,N16)*100</f>
+        <v>29.795918367346943</v>
+      </c>
+    </row>
+    <row r="17" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="4">
+        <v>287</v>
+      </c>
+      <c r="L17">
+        <v>3733</v>
+      </c>
+      <c r="M17">
+        <v>231</v>
+      </c>
+      <c r="N17">
+        <v>709</v>
+      </c>
+      <c r="O17" s="26">
+        <f t="shared" ref="O17:O21" si="6">SUM(K17:L17)/SUM(K17:N17)*100</f>
+        <v>81.048387096774192</v>
+      </c>
+      <c r="P17" s="26">
+        <f t="shared" ref="P17:P21" si="7">K17/SUM(K17+M17)*100</f>
+        <v>55.405405405405403</v>
+      </c>
+      <c r="Q17" s="26">
+        <f t="shared" ref="Q17:Q21" si="8">K17/SUM(K17,N17)*100</f>
+        <v>28.815261044176705</v>
+      </c>
+    </row>
+    <row r="18" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="6">
+        <v>541</v>
+      </c>
+      <c r="L18" s="7">
+        <v>3944</v>
+      </c>
+      <c r="M18" s="7">
+        <v>232</v>
+      </c>
+      <c r="N18" s="7">
+        <v>283</v>
+      </c>
+      <c r="O18" s="27">
+        <f t="shared" si="6"/>
+        <v>89.7</v>
+      </c>
+      <c r="P18" s="27">
+        <f t="shared" si="7"/>
+        <v>69.987063389391977</v>
+      </c>
+      <c r="Q18" s="27">
+        <f t="shared" si="8"/>
+        <v>65.655339805825236</v>
+      </c>
+    </row>
+    <row r="19" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="4">
+        <v>211</v>
+      </c>
+      <c r="L19">
+        <v>4090</v>
+      </c>
+      <c r="M19">
+        <v>151</v>
+      </c>
+      <c r="N19">
+        <v>548</v>
+      </c>
+      <c r="O19" s="26">
+        <f t="shared" si="6"/>
+        <v>86.02</v>
+      </c>
+      <c r="P19" s="26">
+        <f t="shared" si="7"/>
+        <v>58.287292817679557</v>
+      </c>
+      <c r="Q19" s="26">
+        <f t="shared" si="8"/>
+        <v>27.799736495388672</v>
+      </c>
+    </row>
+    <row r="20" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="6">
+        <v>666</v>
+      </c>
+      <c r="L20" s="7">
+        <v>3595</v>
+      </c>
+      <c r="M20" s="7">
+        <v>328</v>
+      </c>
+      <c r="N20" s="7">
+        <v>411</v>
+      </c>
+      <c r="O20" s="27">
+        <f t="shared" si="6"/>
+        <v>85.22</v>
+      </c>
+      <c r="P20" s="27">
+        <f t="shared" si="7"/>
+        <v>67.002012072434596</v>
+      </c>
+      <c r="Q20" s="27">
+        <f t="shared" si="8"/>
+        <v>61.83844011142061</v>
+      </c>
+    </row>
+    <row r="21" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="7">
+        <f>SUM(K16:K20)</f>
+        <v>1778</v>
+      </c>
+      <c r="L21" s="7">
+        <f>SUM(L16:L20)</f>
+        <v>19638</v>
+      </c>
+      <c r="M21" s="7">
+        <f>SUM(M16:M20)</f>
+        <v>971</v>
+      </c>
+      <c r="N21" s="8">
+        <f>SUM(N16:N20)</f>
+        <v>2123</v>
+      </c>
+      <c r="O21" s="27">
+        <f t="shared" si="6"/>
+        <v>87.376580987352099</v>
+      </c>
+      <c r="P21" s="27">
+        <f t="shared" si="7"/>
+        <v>64.678064750818479</v>
+      </c>
+      <c r="Q21" s="27">
+        <f t="shared" si="8"/>
+        <v>45.578056908485003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="J14:Q14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>